<commit_message>
NAICS cluster and SHAP analysis
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriecarey/Documents/projects/2024_05_blog_nn_rand/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57551CFC-25B6-A24C-A595-D06EB4E4F9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C854C7A3-983B-D946-8279-ED12E6F07D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" activeTab="7" xr2:uid="{F11BEE0F-3ECB-0441-A21A-F7FA836E3DFB}"/>
   </bookViews>
@@ -924,7 +924,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -967,6 +967,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2370,7 +2371,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2702,7 +2703,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:G18"/>
+      <selection activeCell="G27" sqref="G27:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3209,10 +3210,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4ADD7A-EA4B-0D4B-B5FC-AB3AD8467496}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3222,7 +3223,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -3286,7 +3287,7 @@
       <c r="C5" s="24">
         <v>0.378485702004141</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="30">
         <v>0.342860739040657</v>
       </c>
       <c r="H5">
@@ -3318,8 +3319,27 @@
       <c r="B7" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+      <c r="C7" s="24">
+        <v>0.37849776924418799</v>
+      </c>
+      <c r="D7" s="30">
+        <v>0.33246456773235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>0.37849776924418799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>0.33246456773235</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="G25" s="10">
+        <v>0.34641051890130498</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>